<commit_message>
CV32E40Pv2: All links updated to cv32e40p_v1.8.3 tag for the 3 target repos (core-v-docs, cv32e40p, core-v-verif).
Signed-off-by: Pascal Gouedo <pascal.gouedo@dolphin.fr>
</commit_message>
<xml_diff>
--- a/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.3/CV32E40Pv2_Design_Issue_Summary.xlsx
+++ b/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.3/CV32E40Pv2_Design_Issue_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\core-v-docs\Project-Descriptions-and-Plans\CV32E40Pv2\Milestone-data\RTL_v1.8.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\core-v-docs\Project-Descriptions-and-Plans\CV32E40Pv2\Milestone-data\RTL_v1.8.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08000072-8359-45AE-8740-073B63E91F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86964ABF-6EC3-4A27-8BFA-6052AC988702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -967,8 +967,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1387,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F34"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1624,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1829,7 +1829,7 @@
       <c r="C16" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="18">
         <v>20</v>
       </c>
       <c r="F16" s="11"/>
@@ -1961,7 +1961,7 @@
       <c r="N23" s="29"/>
     </row>
     <row r="24" spans="2:14" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="6">
+      <c r="B24" s="35">
         <v>169</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -1992,7 +1992,7 @@
       <c r="N24" s="29"/>
     </row>
     <row r="25" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B25" s="6">
+      <c r="B25" s="35">
         <v>170</v>
       </c>
       <c r="C25" s="13" t="s">
@@ -2023,7 +2023,7 @@
       <c r="N25" s="29"/>
     </row>
     <row r="26" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B26" s="6">
+      <c r="B26" s="35">
         <v>174</v>
       </c>
       <c r="C26" s="13" t="s">
@@ -2054,7 +2054,7 @@
       <c r="N26" s="29"/>
     </row>
     <row r="27" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B27" s="6">
+      <c r="B27" s="35">
         <v>197</v>
       </c>
       <c r="C27" s="13" t="s">
@@ -2083,7 +2083,7 @@
       <c r="N27" s="29"/>
     </row>
     <row r="28" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B28" s="6">
+      <c r="B28" s="35">
         <v>252</v>
       </c>
       <c r="C28" s="13" t="s">
@@ -2112,7 +2112,7 @@
       <c r="N28" s="29"/>
     </row>
     <row r="29" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B29" s="6">
+      <c r="B29" s="35">
         <v>308</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -2141,7 +2141,7 @@
       <c r="N29" s="29"/>
     </row>
     <row r="30" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B30" s="6">
+      <c r="B30" s="35">
         <v>452</v>
       </c>
       <c r="C30" s="13" t="s">
@@ -2172,7 +2172,7 @@
       <c r="N30" s="29"/>
     </row>
     <row r="31" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B31" s="6">
+      <c r="B31" s="35">
         <v>462</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -2201,7 +2201,7 @@
       <c r="N31" s="29"/>
     </row>
     <row r="32" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B32" s="6">
+      <c r="B32" s="35">
         <v>571</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -2230,7 +2230,7 @@
       <c r="N32" s="29"/>
     </row>
     <row r="33" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B33" s="6">
+      <c r="B33" s="35">
         <v>598</v>
       </c>
       <c r="C33" s="13" t="s">
@@ -2263,7 +2263,7 @@
       <c r="N33" s="29"/>
     </row>
     <row r="34" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B34" s="6">
+      <c r="B34" s="35">
         <v>599</v>
       </c>
       <c r="C34" s="13" t="s">
@@ -2290,7 +2290,7 @@
       <c r="N34" s="29"/>
     </row>
     <row r="35" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B35" s="6">
+      <c r="B35" s="35">
         <v>600</v>
       </c>
       <c r="C35" s="13" t="s">
@@ -2317,7 +2317,7 @@
       <c r="N35" s="29"/>
     </row>
     <row r="36" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B36" s="6">
+      <c r="B36" s="35">
         <v>605</v>
       </c>
       <c r="C36" s="13" t="s">
@@ -2348,7 +2348,7 @@
       <c r="N36" s="29"/>
     </row>
     <row r="37" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B37" s="6">
+      <c r="B37" s="35">
         <v>606</v>
       </c>
       <c r="C37" s="13" t="s">
@@ -2375,7 +2375,7 @@
       <c r="N37" s="29"/>
     </row>
     <row r="38" spans="2:14" ht="66" x14ac:dyDescent="0.25">
-      <c r="B38" s="6">
+      <c r="B38" s="35">
         <v>612</v>
       </c>
       <c r="C38" s="13" t="s">
@@ -2402,7 +2402,7 @@
       <c r="N38" s="29"/>
     </row>
     <row r="39" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B39" s="6">
+      <c r="B39" s="35">
         <v>629</v>
       </c>
       <c r="C39" s="13" t="s">
@@ -2435,7 +2435,7 @@
       <c r="N39" s="29"/>
     </row>
     <row r="40" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B40" s="6">
+      <c r="B40" s="35">
         <v>650</v>
       </c>
       <c r="C40" s="13" t="s">
@@ -2468,7 +2468,7 @@
       <c r="N40" s="29"/>
     </row>
     <row r="41" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B41" s="6">
+      <c r="B41" s="35">
         <v>652</v>
       </c>
       <c r="C41" s="13" t="s">
@@ -2499,7 +2499,7 @@
       <c r="N41" s="29"/>
     </row>
     <row r="42" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B42" s="6">
+      <c r="B42" s="35">
         <v>663</v>
       </c>
       <c r="C42" s="13" t="s">
@@ -2532,7 +2532,7 @@
       <c r="N42" s="29"/>
     </row>
     <row r="43" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B43" s="6">
+      <c r="B43" s="35">
         <v>670</v>
       </c>
       <c r="C43" s="13" t="s">
@@ -2563,7 +2563,7 @@
       <c r="N43" s="29"/>
     </row>
     <row r="44" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B44" s="6">
+      <c r="B44" s="35">
         <v>684</v>
       </c>
       <c r="C44" s="13" t="s">
@@ -2594,7 +2594,7 @@
       <c r="N44" s="29"/>
     </row>
     <row r="45" spans="2:14" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B45" s="6">
+      <c r="B45" s="35">
         <v>721</v>
       </c>
       <c r="C45" s="13" t="s">
@@ -2621,7 +2621,7 @@
       </c>
     </row>
     <row r="46" spans="2:14" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B46" s="6">
+      <c r="B46" s="35">
         <v>722</v>
       </c>
       <c r="C46" s="13" t="s">
@@ -2648,7 +2648,7 @@
       </c>
     </row>
     <row r="47" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B47" s="6">
+      <c r="B47" s="35">
         <v>723</v>
       </c>
       <c r="C47" s="13" t="s">
@@ -2679,7 +2679,7 @@
       <c r="N47" s="29"/>
     </row>
     <row r="48" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B48" s="6">
+      <c r="B48" s="35">
         <v>724</v>
       </c>
       <c r="C48" s="13" t="s">
@@ -2710,7 +2710,7 @@
       <c r="N48" s="29"/>
     </row>
     <row r="49" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B49" s="6">
+      <c r="B49" s="35">
         <v>725</v>
       </c>
       <c r="C49" s="13" t="s">
@@ -2741,7 +2741,7 @@
       <c r="N49" s="29"/>
     </row>
     <row r="50" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B50" s="6">
+      <c r="B50" s="35">
         <v>726</v>
       </c>
       <c r="C50" s="13" t="s">
@@ -2772,7 +2772,7 @@
       <c r="N50" s="29"/>
     </row>
     <row r="51" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B51" s="6">
+      <c r="B51" s="35">
         <v>727</v>
       </c>
       <c r="C51" s="13" t="s">
@@ -2803,7 +2803,7 @@
       <c r="N51" s="29"/>
     </row>
     <row r="52" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B52" s="6">
+      <c r="B52" s="35">
         <v>728</v>
       </c>
       <c r="C52" s="13" t="s">
@@ -2834,7 +2834,7 @@
       <c r="N52" s="29"/>
     </row>
     <row r="53" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B53" s="6">
+      <c r="B53" s="35">
         <v>729</v>
       </c>
       <c r="C53" s="13" t="s">
@@ -2865,7 +2865,7 @@
       <c r="N53" s="29"/>
     </row>
     <row r="54" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B54" s="6">
+      <c r="B54" s="35">
         <v>730</v>
       </c>
       <c r="C54" s="13" t="s">
@@ -2896,7 +2896,7 @@
       <c r="N54" s="29"/>
     </row>
     <row r="55" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B55" s="6">
+      <c r="B55" s="35">
         <v>731</v>
       </c>
       <c r="C55" s="13" t="s">
@@ -2927,7 +2927,7 @@
       <c r="N55" s="29"/>
     </row>
     <row r="56" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B56" s="6">
+      <c r="B56" s="35">
         <v>741</v>
       </c>
       <c r="C56" s="13" t="s">
@@ -2958,7 +2958,7 @@
       <c r="N56" s="29"/>
     </row>
     <row r="57" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B57" s="6">
+      <c r="B57" s="35">
         <v>742</v>
       </c>
       <c r="C57" s="13" t="s">
@@ -2989,7 +2989,7 @@
       <c r="N57" s="29"/>
     </row>
     <row r="58" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B58" s="6">
+      <c r="B58" s="35">
         <v>756</v>
       </c>
       <c r="C58" s="13" t="s">
@@ -3020,7 +3020,7 @@
       <c r="N58" s="29"/>
     </row>
     <row r="59" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B59" s="6">
+      <c r="B59" s="35">
         <v>800</v>
       </c>
       <c r="C59" s="13" t="s">
@@ -3051,7 +3051,7 @@
       <c r="N59" s="29"/>
     </row>
     <row r="60" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B60" s="6">
+      <c r="B60" s="35">
         <v>838</v>
       </c>
       <c r="C60" s="13" t="s">
@@ -3082,7 +3082,7 @@
       <c r="N60" s="29"/>
     </row>
     <row r="61" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B61" s="6">
+      <c r="B61" s="35">
         <v>840</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -3113,7 +3113,7 @@
       <c r="N61" s="29"/>
     </row>
     <row r="62" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B62" s="6">
+      <c r="B62" s="35">
         <v>850</v>
       </c>
       <c r="C62" s="13" t="s">
@@ -3144,7 +3144,7 @@
       <c r="N62" s="29"/>
     </row>
     <row r="63" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B63" s="6">
+      <c r="B63" s="35">
         <v>862</v>
       </c>
       <c r="C63" s="13" t="s">
@@ -3175,7 +3175,7 @@
       <c r="N63" s="29"/>
     </row>
     <row r="64" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B64" s="6">
+      <c r="B64" s="35">
         <v>869</v>
       </c>
       <c r="C64" s="13" t="s">
@@ -3206,7 +3206,7 @@
       <c r="N64" s="29"/>
     </row>
     <row r="65" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B65" s="6">
+      <c r="B65" s="35">
         <v>870</v>
       </c>
       <c r="C65" s="13" t="s">
@@ -3237,7 +3237,7 @@
       <c r="N65" s="29"/>
     </row>
     <row r="66" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B66" s="6">
+      <c r="B66" s="35">
         <v>876</v>
       </c>
       <c r="C66" s="13" t="s">
@@ -3268,7 +3268,7 @@
       <c r="N66" s="29"/>
     </row>
     <row r="67" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B67" s="6">
+      <c r="B67" s="35">
         <v>877</v>
       </c>
       <c r="C67" s="13" t="s">
@@ -3299,7 +3299,7 @@
       <c r="N67" s="29"/>
     </row>
     <row r="68" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B68" s="6">
+      <c r="B68" s="35">
         <v>880</v>
       </c>
       <c r="C68" s="13" t="s">
@@ -3330,7 +3330,7 @@
       <c r="N68" s="29"/>
     </row>
     <row r="69" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B69" s="6">
+      <c r="B69" s="35">
         <v>887</v>
       </c>
       <c r="C69" s="13" t="s">
@@ -3361,7 +3361,7 @@
       <c r="N69" s="29"/>
     </row>
     <row r="70" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B70" s="6">
+      <c r="B70" s="35">
         <v>888</v>
       </c>
       <c r="C70" s="13" t="s">
@@ -3392,7 +3392,7 @@
       <c r="N70" s="29"/>
     </row>
     <row r="71" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B71" s="6">
+      <c r="B71" s="35">
         <v>889</v>
       </c>
       <c r="C71" s="13" t="s">
@@ -3423,7 +3423,7 @@
       <c r="N71" s="29"/>
     </row>
     <row r="72" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B72" s="6">
+      <c r="B72" s="35">
         <v>894</v>
       </c>
       <c r="C72" s="13" t="s">
@@ -3454,7 +3454,7 @@
       <c r="N72" s="29"/>
     </row>
     <row r="73" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B73" s="6">
+      <c r="B73" s="35">
         <v>896</v>
       </c>
       <c r="C73" s="13" t="s">
@@ -3485,7 +3485,7 @@
       <c r="N73" s="29"/>
     </row>
     <row r="74" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B74" s="6">
+      <c r="B74" s="35">
         <v>901</v>
       </c>
       <c r="C74" s="13" t="s">
@@ -3516,7 +3516,7 @@
       <c r="N74" s="29"/>
     </row>
     <row r="75" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B75" s="6">
+      <c r="B75" s="35">
         <v>959</v>
       </c>
       <c r="C75" s="13" t="s">
@@ -3546,7 +3546,7 @@
       <c r="N75" s="29"/>
     </row>
     <row r="76" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B76" s="6">
+      <c r="B76" s="35">
         <v>960</v>
       </c>
       <c r="C76" s="13" t="s">
@@ -3576,7 +3576,7 @@
       <c r="N76" s="29"/>
     </row>
     <row r="77" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B77" s="6">
+      <c r="B77" s="35">
         <v>965</v>
       </c>
       <c r="C77" s="13" t="s">
@@ -3607,7 +3607,7 @@
       <c r="N77" s="29"/>
     </row>
     <row r="78" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B78" s="6">
+      <c r="B78" s="35">
         <v>975</v>
       </c>
       <c r="C78" s="13" t="s">
@@ -3663,7 +3663,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="F19:F1048576 F1:F2 D3:D18">
+  <conditionalFormatting sqref="F1:F2 D3:D18 F19:F1048576">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Waived">
       <formula>NOT(ISERROR(SEARCH("Waived",D1)))</formula>
     </cfRule>
@@ -3677,6 +3677,63 @@
       <formula>NOT(ISERROR(SEARCH("Not a bug",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B24" r:id="rId1" display="https://github.com/openhwgroup/cv32e40p/issues/169" xr:uid="{3BF811B0-4F05-450E-A175-6DC6D6249BD6}"/>
+    <hyperlink ref="B25" r:id="rId2" display="https://github.com/openhwgroup/cv32e40p/issues/170" xr:uid="{BFEDCAAC-E6D4-4DF6-819E-442ECA2A0720}"/>
+    <hyperlink ref="B26" r:id="rId3" display="https://github.com/openhwgroup/cv32e40p/issues/174" xr:uid="{51A67D76-AD81-419E-8F4E-086530789E34}"/>
+    <hyperlink ref="B27" r:id="rId4" display="https://github.com/openhwgroup/cv32e40p/issues/197" xr:uid="{BBE3A0D1-A9A8-408B-9FC9-53B2F3AC0DCB}"/>
+    <hyperlink ref="B28" r:id="rId5" display="https://github.com/openhwgroup/cv32e40p/issues/252" xr:uid="{01295CFA-67F2-4BB1-AA8B-6A87F9123825}"/>
+    <hyperlink ref="B29" r:id="rId6" display="https://github.com/openhwgroup/cv32e40p/issues/308" xr:uid="{2DDCCB72-FFC9-4DFA-82B7-2762CF464699}"/>
+    <hyperlink ref="B30" r:id="rId7" display="https://github.com/openhwgroup/cv32e40p/issues/452" xr:uid="{CB32CF34-8138-430A-94DC-F10DA1AD6D6D}"/>
+    <hyperlink ref="B31" r:id="rId8" display="https://github.com/openhwgroup/cv32e40p/issues/462" xr:uid="{95FC73EE-FB97-4E18-AB44-DF44BC20BE0D}"/>
+    <hyperlink ref="B32" r:id="rId9" display="https://github.com/openhwgroup/cv32e40p/issues/571" xr:uid="{8AE99A94-15A2-41C3-BBE5-B88E71377E3D}"/>
+    <hyperlink ref="B33" r:id="rId10" display="https://github.com/openhwgroup/cv32e40p/issues/598" xr:uid="{652B05DC-4C26-49C3-8C63-8F8BA5CF4D88}"/>
+    <hyperlink ref="B34" r:id="rId11" display="https://github.com/openhwgroup/cv32e40p/issues/599" xr:uid="{24E0C3FC-C056-4FCE-93B0-250930D3F5F1}"/>
+    <hyperlink ref="B35" r:id="rId12" display="https://github.com/openhwgroup/cv32e40p/issues/600" xr:uid="{717C5424-0904-492D-92A5-BD9A1EA82BCF}"/>
+    <hyperlink ref="B36" r:id="rId13" display="https://github.com/openhwgroup/cv32e40p/issues/605" xr:uid="{46C932B0-A400-45E7-938F-23D394710967}"/>
+    <hyperlink ref="B37" r:id="rId14" display="https://github.com/openhwgroup/cv32e40p/issues/606" xr:uid="{A373B945-EC2A-4933-A986-A5D7605C8BB0}"/>
+    <hyperlink ref="B38" r:id="rId15" display="https://github.com/openhwgroup/cv32e40p/issues/612" xr:uid="{822CB0A7-3119-4438-937E-F9782F3E4F4B}"/>
+    <hyperlink ref="B39" r:id="rId16" display="https://github.com/openhwgroup/cv32e40p/issues/629" xr:uid="{BF00CB44-04A6-48E4-83B4-94017A671CB7}"/>
+    <hyperlink ref="B40" r:id="rId17" display="https://github.com/openhwgroup/cv32e40p/issues/650" xr:uid="{143B46F5-64F9-4656-9C58-FE2BA3366829}"/>
+    <hyperlink ref="B41" r:id="rId18" display="https://github.com/openhwgroup/cv32e40p/issues/652" xr:uid="{9B811422-8337-4EEB-978A-647CE9ED1872}"/>
+    <hyperlink ref="B42" r:id="rId19" display="https://github.com/openhwgroup/cv32e40p/issues/663" xr:uid="{8237B572-C80A-4253-81CA-1A3C58350B0A}"/>
+    <hyperlink ref="B43" r:id="rId20" display="https://github.com/openhwgroup/cv32e40p/issues/670" xr:uid="{8C9826CF-68BF-46B7-9840-3349B9F8105F}"/>
+    <hyperlink ref="B44" r:id="rId21" display="https://github.com/openhwgroup/cv32e40p/issues/684" xr:uid="{47F1066C-0F28-458B-8C3F-E24D16D631E5}"/>
+    <hyperlink ref="B45" r:id="rId22" display="https://github.com/openhwgroup/cv32e40p/issues/721" xr:uid="{4E8FDA1A-D055-40AE-AA20-3901043ACA07}"/>
+    <hyperlink ref="B46" r:id="rId23" display="https://github.com/openhwgroup/cv32e40p/issues/722" xr:uid="{A9AB69EB-B28C-43DB-9691-7CA40726A014}"/>
+    <hyperlink ref="B47" r:id="rId24" display="https://github.com/openhwgroup/cv32e40p/issues/723" xr:uid="{9B109156-BF47-455B-91C6-6E28A9B39887}"/>
+    <hyperlink ref="B48" r:id="rId25" display="https://github.com/openhwgroup/cv32e40p/issues/724" xr:uid="{70457381-FC2A-467E-8124-805FE9053AB4}"/>
+    <hyperlink ref="B49" r:id="rId26" display="https://github.com/openhwgroup/cv32e40p/issues/725" xr:uid="{62939D3B-73D9-4421-BE42-96477CF8C463}"/>
+    <hyperlink ref="B50" r:id="rId27" display="https://github.com/openhwgroup/cv32e40p/issues/726" xr:uid="{0AB0FBC0-28AF-4965-B60F-B54B69041783}"/>
+    <hyperlink ref="B51" r:id="rId28" display="https://github.com/openhwgroup/cv32e40p/issues/727" xr:uid="{500E3377-557B-4844-898A-FFFDB770C190}"/>
+    <hyperlink ref="B52" r:id="rId29" display="https://github.com/openhwgroup/cv32e40p/issues/728" xr:uid="{6FC77E4B-80A7-4BDE-9310-AE14415233E3}"/>
+    <hyperlink ref="B53" r:id="rId30" display="https://github.com/openhwgroup/cv32e40p/issues/729" xr:uid="{9C1DD66C-5D00-4E26-B6A0-7AA73AEC2837}"/>
+    <hyperlink ref="B54" r:id="rId31" display="https://github.com/openhwgroup/cv32e40p/issues/730" xr:uid="{BD2360C3-6866-403B-BFF2-EA83F796285B}"/>
+    <hyperlink ref="B55" r:id="rId32" display="https://github.com/openhwgroup/cv32e40p/issues/731" xr:uid="{A0A625B9-110A-44D4-BAAF-110A42C17920}"/>
+    <hyperlink ref="B56" r:id="rId33" display="https://github.com/openhwgroup/cv32e40p/issues/741" xr:uid="{C4787077-B147-4C77-B05F-70F95927678D}"/>
+    <hyperlink ref="B57" r:id="rId34" display="https://github.com/openhwgroup/cv32e40p/issues/742" xr:uid="{C04E6E71-A1D7-44C9-834E-1261CA2AAAB9}"/>
+    <hyperlink ref="B58" r:id="rId35" display="https://github.com/openhwgroup/cv32e40p/issues/756" xr:uid="{C6B465E1-AD85-440D-A7F1-E6D9AC949AE8}"/>
+    <hyperlink ref="B59" r:id="rId36" display="https://github.com/openhwgroup/cv32e40p/issues/800" xr:uid="{70131C65-4484-4C14-9CBC-ABE34C3E8D33}"/>
+    <hyperlink ref="B60" r:id="rId37" display="https://github.com/openhwgroup/cv32e40p/issues/838" xr:uid="{32A5204A-626C-421F-B9CD-7E00F4681919}"/>
+    <hyperlink ref="B61" r:id="rId38" display="https://github.com/openhwgroup/cv32e40p/issues/840" xr:uid="{489A0E0C-37D9-4334-A077-E7984255CDEF}"/>
+    <hyperlink ref="B62" r:id="rId39" display="https://github.com/openhwgroup/cv32e40p/issues/850" xr:uid="{8B5B9C51-E0FE-4BA6-ADB5-BF4399211BE6}"/>
+    <hyperlink ref="B63" r:id="rId40" display="https://github.com/openhwgroup/cv32e40p/issues/862" xr:uid="{0EDCAAF7-672D-41E9-B4EB-6F04AE78BD7C}"/>
+    <hyperlink ref="B64" r:id="rId41" display="https://github.com/openhwgroup/cv32e40p/issues/869" xr:uid="{3EC66B25-CF8E-4FA1-B44B-8AF7B60C8E18}"/>
+    <hyperlink ref="B65" r:id="rId42" display="https://github.com/openhwgroup/cv32e40p/issues/870" xr:uid="{4ACB4F68-A87D-490D-A8D0-346A7992CCC7}"/>
+    <hyperlink ref="B66" r:id="rId43" display="https://github.com/openhwgroup/cv32e40p/issues/876" xr:uid="{BA9C69BF-0A82-452D-842D-20DD8FE62F9C}"/>
+    <hyperlink ref="B67" r:id="rId44" display="https://github.com/openhwgroup/cv32e40p/issues/877" xr:uid="{F1A234EE-1772-42B9-9678-5FB272CFAD29}"/>
+    <hyperlink ref="B68" r:id="rId45" display="https://github.com/openhwgroup/cv32e40p/issues/880" xr:uid="{9F609482-AA28-4A4C-8DA9-AE3A0C1153A4}"/>
+    <hyperlink ref="B69" r:id="rId46" display="https://github.com/openhwgroup/cv32e40p/issues/887" xr:uid="{E8A38474-EA04-427D-B27F-CB8C2DDD4D35}"/>
+    <hyperlink ref="B70" r:id="rId47" display="https://github.com/openhwgroup/cv32e40p/issues/888" xr:uid="{A6124B86-0823-4BD8-9746-E6767715D088}"/>
+    <hyperlink ref="B71" r:id="rId48" display="https://github.com/openhwgroup/cv32e40p/issues/889" xr:uid="{4578FFA2-9298-46B2-851B-F5C46FBC5EF0}"/>
+    <hyperlink ref="B72" r:id="rId49" display="https://github.com/openhwgroup/cv32e40p/issues/894" xr:uid="{CB4BD25C-F7BA-47FB-9470-7B368AEF8F41}"/>
+    <hyperlink ref="B73" r:id="rId50" display="https://github.com/openhwgroup/cv32e40p/issues/896" xr:uid="{C43D7F4B-5C18-4932-BAC3-66B6A444DE95}"/>
+    <hyperlink ref="B74" r:id="rId51" display="https://github.com/openhwgroup/cv32e40p/issues/901" xr:uid="{39AF59DE-E8DA-419B-9E8E-2139FC6B285E}"/>
+    <hyperlink ref="B75" r:id="rId52" display="https://github.com/openhwgroup/cv32e40p/issues/959" xr:uid="{C0E03DF6-1DED-40A0-B511-D900689D8E34}"/>
+    <hyperlink ref="B76" r:id="rId53" display="https://github.com/openhwgroup/cv32e40p/issues/960" xr:uid="{16007D1D-50BF-42A4-BE78-4A159E807EEB}"/>
+    <hyperlink ref="B77" r:id="rId54" display="https://github.com/openhwgroup/cv32e40p/issues/965" xr:uid="{CF107A18-EFB4-4602-B078-25BF2B033F43}"/>
+    <hyperlink ref="B78" r:id="rId55" display="https://github.com/openhwgroup/cv32e40p/issues/975" xr:uid="{75CE9E28-3E62-4BDF-B62D-8AF5DF95CCAC}"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -3687,21 +3744,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
-    <SharedWithUsers xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3954,21 +4002,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
+    <SharedWithUsers xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A65D6B25-B4CF-4DD2-B0D1-F3288A654A97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76AFA4A-AF05-419D-BE9B-332D578E982D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
-    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3993,9 +4047,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76AFA4A-AF05-419D-BE9B-332D578E982D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A65D6B25-B4CF-4DD2-B0D1-F3288A654A97}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
+    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>